<commit_message>
Sprint 1 Week 1 deliverable
</commit_message>
<xml_diff>
--- a/scrum/sprint1/s1_burndown.xlsx
+++ b/scrum/sprint1/s1_burndown.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21140" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>ideal</t>
   </si>
@@ -33,9 +33,6 @@
     <t>Person</t>
   </si>
   <si>
-    <t>Hours</t>
-  </si>
-  <si>
     <t>Ryan</t>
   </si>
   <si>
@@ -64,6 +61,39 @@
   </si>
   <si>
     <t>Ryan Ordille</t>
+  </si>
+  <si>
+    <t>Estimated Hours</t>
+  </si>
+  <si>
+    <t>finished</t>
+  </si>
+  <si>
+    <t>hours remaining (at start of day)</t>
+  </si>
+  <si>
+    <t>actual hours</t>
+  </si>
+  <si>
+    <t>week 1</t>
+  </si>
+  <si>
+    <t>week 3</t>
+  </si>
+  <si>
+    <t>week 2</t>
+  </si>
+  <si>
+    <t>sprint 1</t>
+  </si>
+  <si>
+    <t>TODO:</t>
+  </si>
+  <si>
+    <t>convert real entries to day before minus finished</t>
+  </si>
+  <si>
+    <t>Team McBuddy</t>
   </si>
 </sst>
 </file>
@@ -432,6 +462,30 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="22"/>
+                <c:pt idx="0">
+                  <c:v>105.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>103.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>103.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>103.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>98.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>90.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>85.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>83.0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -447,11 +501,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2145222632"/>
-        <c:axId val="2144421032"/>
+        <c:axId val="2066841016"/>
+        <c:axId val="2065942968"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="2145222632"/>
+        <c:axId val="2066841016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -485,14 +539,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2144421032"/>
+        <c:crossAx val="2065942968"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="2144421032"/>
+        <c:axId val="2065942968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -522,7 +576,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2145222632"/>
+        <c:crossAx val="2066841016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -548,15 +602,15 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>673100</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>63500</xdr:colOff>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>25400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>88900</xdr:colOff>
-      <xdr:row>41</xdr:row>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>49</xdr:row>
       <xdr:rowOff>25400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -901,14 +955,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:W19"/>
+  <dimension ref="A1:W27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P15" sqref="P15"/>
+      <selection activeCell="V9" sqref="V9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
+    <row r="1" spans="1:23">
+      <c r="D1" t="s">
+        <v>16</v>
+      </c>
+    </row>
     <row r="2" spans="1:23">
       <c r="B2" s="1">
         <v>42023</v>
@@ -1052,43 +1111,119 @@
       <c r="A4" t="s">
         <v>1</v>
       </c>
+      <c r="B4">
+        <v>105</v>
+      </c>
+      <c r="C4">
+        <v>103</v>
+      </c>
+      <c r="D4">
+        <v>103</v>
+      </c>
+      <c r="E4">
+        <v>103</v>
+      </c>
+      <c r="F4">
+        <v>98</v>
+      </c>
+      <c r="G4">
+        <v>90</v>
+      </c>
+      <c r="H4">
+        <v>85</v>
+      </c>
+      <c r="I4">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>5</v>
+      </c>
+      <c r="F6">
+        <v>8</v>
+      </c>
+      <c r="G6">
+        <v>5</v>
+      </c>
+      <c r="H6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23">
+      <c r="C9" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="10" spans="1:23">
       <c r="A10" t="s">
         <v>3</v>
       </c>
       <c r="B10" t="s">
-        <v>4</v>
+        <v>14</v>
+      </c>
+      <c r="C10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" t="s">
+        <v>19</v>
+      </c>
+      <c r="F10" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:23">
       <c r="A11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B11">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="C11">
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:23">
       <c r="A12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B12">
         <v>12</v>
       </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
       <c r="P12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:23">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B13">
         <v>11</v>
       </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
       <c r="P13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:23">
@@ -1098,46 +1233,78 @@
       <c r="B14">
         <v>12</v>
       </c>
+      <c r="C14">
+        <v>7</v>
+      </c>
+      <c r="P14" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="15" spans="1:23">
       <c r="A15" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B15">
         <v>12</v>
       </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:23">
       <c r="A16" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B16">
         <v>11</v>
       </c>
-    </row>
-    <row r="17" spans="1:2">
+      <c r="C16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B17">
         <v>24</v>
       </c>
-    </row>
-    <row r="18" spans="1:2">
+      <c r="C17">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B18">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
+        <v>11</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B19">
         <f>SUM(B11:B18)</f>
         <v>105</v>
+      </c>
+      <c r="C19">
+        <f>SUM(C11:C18)</f>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>